<commit_message>
docker compose for auth server
</commit_message>
<xml_diff>
--- a/data/insert_data.xlsx
+++ b/data/insert_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kongh\Desktop\DATN\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA4E329-A019-427A-B081-456E977D28F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C38970-DD1C-4EF6-91DE-2DBDFA89DD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3D981FB0-44E2-41B7-9F67-DB59F3D45F24}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
demo add and edit Actites
</commit_message>
<xml_diff>
--- a/data/insert_data.xlsx
+++ b/data/insert_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEAMWORKING\Final\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2A4A5A-F60D-44EE-9B94-89F9170AAD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792AE409-5454-437B-9734-813421B4C089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3D981FB0-44E2-41B7-9F67-DB59F3D45F24}"/>
   </bookViews>
@@ -632,7 +632,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>